<commit_message>
Removed PoiFormulaHelper - Moved original PoiFormulaHelper methods into the model element classes themselves - Added test resources - Added convenience fields for model element types
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF0DF72-8A81-0941-A645-327D23B160EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347DFD8B-D143-A340-9C68-71888E3B7EF0}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-76800" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
+    <workbookView xWindow="-76800" yWindow="460" windowWidth="19200" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
   <sheets>
-    <sheet name="PoiFormulaHelperTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="ExcelFormulaTreeTest" sheetId="1" r:id="rId1"/>
+    <sheet name="Lookup" sheetId="3" r:id="rId2"/>
+    <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,113 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+  <si>
+    <t>Arithmetic no brackets</t>
+  </si>
+  <si>
+    <t>Arithmetic 1 bracket</t>
+  </si>
+  <si>
+    <t>Arithmetic 1 bracket variation</t>
+  </si>
+  <si>
+    <t>Aritmetic 2 sets of brackets</t>
+  </si>
+  <si>
+    <t>SUM over 1 operand or</t>
+  </si>
+  <si>
+    <t>SUM over multiple operands</t>
+  </si>
+  <si>
+    <t>Unary operation formula</t>
+  </si>
+  <si>
+    <t>Percentage formula</t>
+  </si>
+  <si>
+    <t>Multiple Function Eval</t>
+  </si>
+  <si>
+    <t>VLOOKUP</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
+  </si>
+  <si>
+    <t>C1 Result</t>
+  </si>
+  <si>
+    <t>D1 Result</t>
+  </si>
+  <si>
+    <t>E1 Result</t>
+  </si>
+  <si>
+    <t>B1 Result</t>
+  </si>
+  <si>
+    <t>B2 Result</t>
+  </si>
+  <si>
+    <t>C2 Result</t>
+  </si>
+  <si>
+    <t>D2 Result</t>
+  </si>
+  <si>
+    <t>E2 Result</t>
+  </si>
+  <si>
+    <t>B3 Result</t>
+  </si>
+  <si>
+    <t>C3 Result</t>
+  </si>
+  <si>
+    <t>D3 Result</t>
+  </si>
+  <si>
+    <t>E3 Result</t>
+  </si>
+  <si>
+    <t>B4 Result</t>
+  </si>
+  <si>
+    <t>C4 Result</t>
+  </si>
+  <si>
+    <t>D4 Result</t>
+  </si>
+  <si>
+    <t>E4 Result</t>
+  </si>
+  <si>
+    <t>B5 Result</t>
+  </si>
+  <si>
+    <t>C5 Result</t>
+  </si>
+  <si>
+    <t>D5 Result</t>
+  </si>
+  <si>
+    <t>E5 Result</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -376,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252C82E-34D7-43AB-88EB-EAE289BCD8A4}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -387,16 +494,100 @@
     <col min="1" max="1" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1">
         <f>SUM(Data!A1:D5)</f>
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <f>SUM(Data!B1,Data!D5,Data!B5,Data!D2,Data!C2)</f>
         <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <f>65+20</f>
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f>(6*5)+500</f>
+        <v>530</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f>6*(5+500)</f>
+        <v>3030</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f>(34*45)+(800/40)</f>
+        <v>1550</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f>-(8-4)</f>
+        <v>-4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f>9%</f>
+        <v>0.09</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>SUM(Data!A1:D5)+SUM(Data!B1:D5)</f>
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="str">
+        <f>VLOOKUP("A1", Lookup!A1:E5, 3)</f>
+        <v>C1 Result</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="str">
+        <f>VLOOKUP("A2", Lookup!A1:E5, 3)</f>
+        <v>C2 Result</v>
       </c>
     </row>
   </sheetData>
@@ -405,11 +596,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6459477B-C2F1-614F-A293-DF72F94DA95A}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF83E4A6-19CF-4ACC-A332-CE2869C6C216}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated AiLookup to return SheetName rather than SheetIndex - Added reference to calling ExcelBook for AI functions - Changed visibility of evaluator in ExcelBook - Changed instance management of AiFunctions aggregator
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F40AB5-A33E-DC42-865A-6DAD7762AF2D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3887B2F4-DCE0-B34E-9C64-087FEBE19E79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelFormulaTreeTest" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Arithmetic no brackets</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Abstract Interpretation</t>
-  </si>
-  <si>
-    <t>PercentPtg</t>
   </si>
 </sst>
 </file>
@@ -173,8 +170,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -492,7 +490,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -520,9 +518,9 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" t="str">
-        <f>VLOOKUP("A1", CHOOSE(2, A1:B5, Lookup!A1:F5), 600%)</f>
-        <v>PercentPtg</v>
+      <c r="H2">
+        <f>MATCH("A1", Lookup!A1:A5)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -610,104 +608,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6459477B-C2F1-614F-A293-DF72F94DA95A}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="R25" sqref="F1:R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Refactored parse tree builder to take into account optimised FUNCTIONS that use skip tokens
</commit_message>
<xml_diff>
--- a/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
+++ b/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/ExcelFormulaTreeTest.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/ws-epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonathanco/repos/epsilon/emc-cellsheet/tests/org.eclipse.epsilon.emc.cellsheet.excel.tests/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3887B2F4-DCE0-B34E-9C64-087FEBE19E79}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF01D972-A42A-8848-85FB-15835D00EBE2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{89D4AF0C-424F-4474-A077-5A7CAA947044}"/>
   </bookViews>
   <sheets>
     <sheet name="ExcelFormulaTreeTest" sheetId="1" r:id="rId1"/>
     <sheet name="Lookup" sheetId="3" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -487,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4252C82E-34D7-43AB-88EB-EAE289BCD8A4}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="E12" sqref="C12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -601,6 +606,27 @@
         <v>C2 Result</v>
       </c>
     </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="b">
+        <f>IF(E12&gt;(1+50),C12,D12)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="str">
+        <f>IF(E12&gt;0,"Yes")</f>
+        <v>Yes</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -611,7 +637,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R25" sqref="F1:R25"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>